<commit_message>
took big boss changes and this contains all test DE Code fix
</commit_message>
<xml_diff>
--- a/dataFiles/test_schema_files/SNDREV.W5PA_TestSchema.xlsx
+++ b/dataFiles/test_schema_files/SNDREV.W5PA_TestSchema.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://riversideassessments-my.sharepoint.com/personal/martin_vondruska_riversideinsights_com/Documents/WJ V Clinical Development/Final Content for ENG_Publication/SNDREV - Sound Reversal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanteteg\Documents\Riverside\Manuscript Updates\Manuscript Changes to Aneta\SNDREV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{590091E6-6948-4ED5-9C06-40F58B489BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E262016E-81D7-42E0-9A28-CA5B8E9C7FD0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF163ACF-DC2B-4606-ADB8-5DB3DA3BF2CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="60" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{83B6147D-AEDB-4F3F-8015-C6928745C0B9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{83B6147D-AEDB-4F3F-8015-C6928745C0B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scheme" sheetId="1" r:id="rId1"/>
     <sheet name="Edit Tracker" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Scheme'!$A$1:$AG$604</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Test Scheme'!$A$1:$AD$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Scheme'!$A$1:$AG$603</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Test Scheme'!$A$1:$AD$29</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="223">
   <si>
     <t>Form</t>
   </si>
@@ -955,15 +955,6 @@
     <t>SNDREV_020</t>
   </si>
   <si>
-    <t>snake</t>
-  </si>
-  <si>
-    <t>snake-canes</t>
-  </si>
-  <si>
-    <t>canes</t>
-  </si>
-  <si>
     <t>23</t>
   </si>
   <si>
@@ -985,9 +976,6 @@
     <t>24</t>
   </si>
   <si>
-    <t>Item 21</t>
-  </si>
-  <si>
     <t>SNDREV_030</t>
   </si>
   <si>
@@ -998,9 +986,6 @@
   </si>
   <si>
     <t>funny</t>
-  </si>
-  <si>
-    <t>25</t>
   </si>
   <si>
     <t xml:space="preserve"> SNDREV_QOP</t>
@@ -1186,6 +1171,12 @@
   </si>
   <si>
     <t>Sample A, Trial 2</t>
+  </si>
+  <si>
+    <t>GJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Based on in info in UAT Tracker and Issues Log and previous AU request (from 4/12/2024), removed Item 19 "snake." Added to list (to the right on this screen). Updated manuscript for a total of 20 test items. Next step: update valid WLookup Score Range to 0-20 in US (JLC). </t>
   </si>
 </sst>
 </file>
@@ -1898,12 +1889,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AG604"/>
+  <dimension ref="A1:AG603"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="N1" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2034,7 +2025,7 @@
         <v>29</v>
       </c>
       <c r="AE1" s="47" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>30</v>
@@ -2066,7 +2057,7 @@
         <v>36</v>
       </c>
       <c r="H2" s="53" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="I2" s="18" t="s">
         <v>37</v>
@@ -2155,7 +2146,7 @@
         <v>41</v>
       </c>
       <c r="H3" s="53" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I3" s="18" t="s">
         <v>42</v>
@@ -2250,7 +2241,7 @@
         <v>51</v>
       </c>
       <c r="H4" s="53" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="I4" s="18" t="s">
         <v>53</v>
@@ -2735,7 +2726,7 @@
         <v>38</v>
       </c>
       <c r="N9" s="25" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="O9" s="29" t="s">
         <v>83</v>
@@ -4030,14 +4021,14 @@
       <c r="A23" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="29" t="s">
         <v>163</v>
       </c>
       <c r="C23" s="45">
-        <v>426908943</v>
+        <v>426908564</v>
       </c>
       <c r="D23" s="48">
-        <v>552953673</v>
+        <v>552961584</v>
       </c>
       <c r="E23" s="31" t="s">
         <v>34</v>
@@ -4045,14 +4036,14 @@
       <c r="F23" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G23" s="18" t="s">
+      <c r="G23" s="31" t="s">
         <v>164</v>
       </c>
       <c r="H23" s="53" t="s">
         <v>164</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="J23" s="44"/>
       <c r="K23" s="18" t="s">
@@ -4065,13 +4056,13 @@
         <v>38</v>
       </c>
       <c r="N23" s="23" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="O23" s="29" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="P23" s="17" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="Q23" s="18" t="s">
         <v>46</v>
@@ -4125,14 +4116,14 @@
       <c r="A24" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>169</v>
+      <c r="B24" s="29" t="s">
+        <v>166</v>
       </c>
       <c r="C24" s="45">
-        <v>426908564</v>
+        <v>426910913</v>
       </c>
       <c r="D24" s="48">
-        <v>552961584</v>
+        <v>552963457</v>
       </c>
       <c r="E24" s="31" t="s">
         <v>34</v>
@@ -4140,14 +4131,14 @@
       <c r="F24" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G24" s="18" t="s">
-        <v>170</v>
+      <c r="G24" s="31" t="s">
+        <v>167</v>
       </c>
       <c r="H24" s="53" t="s">
-        <v>170</v>
-      </c>
-      <c r="I24" s="18" t="s">
-        <v>171</v>
+        <v>167</v>
+      </c>
+      <c r="I24" s="43" t="s">
+        <v>173</v>
       </c>
       <c r="J24" s="44"/>
       <c r="K24" s="18" t="s">
@@ -4160,13 +4151,13 @@
         <v>38</v>
       </c>
       <c r="N24" s="23" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="O24" s="29" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="P24" s="17" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="Q24" s="18" t="s">
         <v>46</v>
@@ -4216,151 +4207,91 @@
       </c>
       <c r="AG24" s="17"/>
     </row>
-    <row r="25" spans="1:33" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="17" t="s">
+    <row r="25" spans="1:33" s="12" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="C25" s="45">
-        <v>426910913</v>
-      </c>
-      <c r="D25" s="48">
-        <v>552963457</v>
-      </c>
-      <c r="E25" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="H25" s="53" t="s">
-        <v>176</v>
-      </c>
-      <c r="I25" s="43" t="s">
+      <c r="B25" s="29" t="s">
+        <v>172</v>
+      </c>
+      <c r="C25" s="30">
+        <v>443231720</v>
+      </c>
+      <c r="D25" s="51" t="s">
+        <v>214</v>
+      </c>
+      <c r="E25" s="31"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="J25" s="44"/>
-      <c r="K25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="L25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="M25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="N25" s="23" t="s">
+      <c r="J25" s="42"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="O25" s="29" t="s">
+      <c r="O25" s="29"/>
+      <c r="P25" s="29"/>
+      <c r="Q25" s="31"/>
+      <c r="R25" s="31"/>
+      <c r="S25" s="31"/>
+      <c r="T25" s="31"/>
+      <c r="U25" s="31"/>
+      <c r="V25" s="31"/>
+      <c r="W25" s="31"/>
+      <c r="X25" s="31"/>
+      <c r="Y25" s="31"/>
+      <c r="Z25" s="31"/>
+      <c r="AA25" s="31"/>
+      <c r="AB25" s="31"/>
+      <c r="AC25" s="31"/>
+      <c r="AD25" s="31"/>
+      <c r="AE25" s="31"/>
+      <c r="AF25" s="31" t="s">
         <v>179</v>
       </c>
-      <c r="P25" s="17" t="s">
+      <c r="AG25" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="Q25" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="R25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="S25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="T25" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="U25" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="V25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="W25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="X25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE25" s="18"/>
-      <c r="AF25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="AG25" s="17"/>
-    </row>
-    <row r="26" spans="1:33" s="12" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="29" t="s">
-        <v>181</v>
-      </c>
-      <c r="C26" s="30">
-        <v>443231720</v>
-      </c>
-      <c r="D26" s="51" t="s">
-        <v>219</v>
-      </c>
-      <c r="E26" s="31"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="41" t="s">
-        <v>182</v>
-      </c>
-      <c r="J26" s="42"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="32" t="s">
-        <v>183</v>
-      </c>
-      <c r="O26" s="29"/>
-      <c r="P26" s="29"/>
-      <c r="Q26" s="31"/>
-      <c r="R26" s="31"/>
-      <c r="S26" s="31"/>
-      <c r="T26" s="31"/>
-      <c r="U26" s="31"/>
-      <c r="V26" s="31"/>
-      <c r="W26" s="31"/>
-      <c r="X26" s="31"/>
-      <c r="Y26" s="31"/>
-      <c r="Z26" s="31"/>
-      <c r="AA26" s="31"/>
-      <c r="AB26" s="31"/>
-      <c r="AC26" s="31"/>
-      <c r="AD26" s="31"/>
-      <c r="AE26" s="31"/>
-      <c r="AF26" s="31" t="s">
-        <v>184</v>
-      </c>
-      <c r="AG26" s="46" t="s">
-        <v>185</v>
-      </c>
+    </row>
+    <row r="26" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
+      <c r="U26" s="12"/>
+      <c r="V26" s="12"/>
+      <c r="W26" s="12"/>
+      <c r="X26" s="12"/>
+      <c r="Y26" s="12"/>
+      <c r="Z26" s="12"/>
+      <c r="AA26" s="12"/>
+      <c r="AB26" s="12"/>
+      <c r="AC26" s="12"/>
+      <c r="AD26" s="12"/>
+      <c r="AE26" s="12"/>
+      <c r="AF26" s="12"/>
+      <c r="AG26" s="12"/>
     </row>
     <row r="27" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10"/>
@@ -4614,33 +4545,12 @@
       <c r="D34" s="49"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="12"/>
-      <c r="P34" s="10"/>
-      <c r="Q34" s="12"/>
-      <c r="R34" s="12"/>
-      <c r="S34" s="12"/>
-      <c r="T34" s="12"/>
-      <c r="U34" s="12"/>
-      <c r="V34" s="12"/>
-      <c r="W34" s="12"/>
-      <c r="X34" s="12"/>
-      <c r="Y34" s="12"/>
-      <c r="Z34" s="12"/>
-      <c r="AA34" s="12"/>
-      <c r="AB34" s="12"/>
-      <c r="AC34" s="12"/>
-      <c r="AD34" s="12"/>
-      <c r="AE34" s="12"/>
-      <c r="AF34" s="12"/>
-      <c r="AG34" s="12"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="N34" s="9"/>
+      <c r="P34" s="11"/>
     </row>
     <row r="35" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="10"/>
@@ -12608,22 +12518,8 @@
       <c r="N603" s="9"/>
       <c r="P603" s="11"/>
     </row>
-    <row r="604" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A604" s="10"/>
-      <c r="B604" s="10"/>
-      <c r="C604" s="10"/>
-      <c r="D604" s="49"/>
-      <c r="E604" s="10"/>
-      <c r="F604" s="10"/>
-      <c r="I604" s="11"/>
-      <c r="J604" s="11"/>
-      <c r="K604" s="11"/>
-      <c r="L604" s="11"/>
-      <c r="N604" s="9"/>
-      <c r="P604" s="11"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:AG604" xr:uid="{889C9C9A-F5C9-4AEE-AFAB-473C7B2118CF}"/>
+  <autoFilter ref="A1:AG603" xr:uid="{889C9C9A-F5C9-4AEE-AFAB-473C7B2118CF}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="27" fitToHeight="0" orientation="landscape" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -12632,11 +12528,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B7561C4-6331-4A7B-80FF-F338DFD70F93}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12653,47 +12549,47 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B2" s="16">
         <v>44319</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B3" s="16">
         <v>44508</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D3" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E3" s="16">
         <v>44510</v>
@@ -12701,16 +12597,16 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B4" s="16">
         <v>44508</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D4" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E4" s="16">
         <v>44510</v>
@@ -12718,16 +12614,16 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B5" s="16">
         <v>44508</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D5" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E5" s="16">
         <v>44510</v>
@@ -12735,36 +12631,36 @@
     </row>
     <row r="6" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B6" s="16">
         <v>44508</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E6" s="16">
         <v>44510</v>
       </c>
       <c r="F6" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B7" s="16">
         <v>44524</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D7" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E7" s="16">
         <v>44529</v>
@@ -12772,16 +12668,16 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B8" s="16">
         <v>44524</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D8" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E8" s="16">
         <v>44529</v>
@@ -12789,16 +12685,16 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B9" s="16">
         <v>44524</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D9" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E9" s="16">
         <v>44529</v>
@@ -12806,16 +12702,16 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B10" s="16">
         <v>44524</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D10" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E10" s="16">
         <v>44529</v>
@@ -12823,16 +12719,16 @@
     </row>
     <row r="11" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B11" s="16">
         <v>44524</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D11" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E11" s="16">
         <v>44529</v>
@@ -12840,16 +12736,16 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B12" s="16">
         <v>44524</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D12" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E12" s="16">
         <v>44529</v>
@@ -12864,29 +12760,29 @@
     </row>
     <row r="14" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B14" s="16">
         <v>45219</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D14" s="33"/>
       <c r="E14" s="33"/>
       <c r="F14" s="13" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B15" s="16">
         <v>45223</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
@@ -12903,13 +12799,13 @@
     </row>
     <row r="16" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B16" s="16">
         <v>45240</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D16" s="33"/>
       <c r="E16" s="33"/>
@@ -12920,19 +12816,19 @@
         <v>92</v>
       </c>
       <c r="H16" s="38" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="M16" s="36"/>
     </row>
     <row r="17" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B17" s="16">
         <v>45245</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F17" s="24">
         <v>426883919</v>
@@ -12941,19 +12837,19 @@
         <v>122</v>
       </c>
       <c r="H17" s="38" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="M17" s="36"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B18" s="16">
         <v>45245</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="F18" s="24">
         <v>426891896</v>
@@ -12962,19 +12858,19 @@
         <v>140</v>
       </c>
       <c r="H18" s="38" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="M18" s="39"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B19" s="16">
         <v>45245</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="F19" s="24">
         <v>426898679</v>
@@ -12983,24 +12879,38 @@
         <v>158</v>
       </c>
       <c r="H19" s="38" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B20" s="16">
         <v>45258</v>
       </c>
       <c r="C20" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="F20" s="45">
+        <v>426908943</v>
+      </c>
+      <c r="G20" s="53" t="s">
+        <v>164</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>221</v>
+      </c>
+      <c r="B21" s="16">
+        <v>45464</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D20" t="s">
-        <v>193</v>
-      </c>
-      <c r="E20" s="16">
-        <v>45259</v>
       </c>
     </row>
   </sheetData>
@@ -13009,12 +12919,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ACB55C607407B649B58320C323E134CB" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c13994d6d2ddba02aa5dd940c3aa9f4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fb8057a2-d102-4556-bf3d-1bd060c1c6e1" xmlns:ns4="3fbd1978-31ec-4369-8fe8-e6440116bc51" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fff83f4678cd9c540a9875a311617aea" ns3:_="" ns4:_="">
     <xsd:import namespace="fb8057a2-d102-4556-bf3d-1bd060c1c6e1"/>
@@ -13237,7 +13141,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -13246,16 +13150,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB7C9551-4A2B-4721-89B5-925D245FA51E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{873E718D-0E51-406D-B7BE-C3027393B741}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13274,10 +13175,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{802F3D32-8F37-45EF-8DEF-C7FB26649453}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB7C9551-4A2B-4721-89B5-925D245FA51E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
took big boss changes and this contains all test DE Code fix (#44)
</commit_message>
<xml_diff>
--- a/dataFiles/test_schema_files/SNDREV.W5PA_TestSchema.xlsx
+++ b/dataFiles/test_schema_files/SNDREV.W5PA_TestSchema.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://riversideassessments-my.sharepoint.com/personal/martin_vondruska_riversideinsights_com/Documents/WJ V Clinical Development/Final Content for ENG_Publication/SNDREV - Sound Reversal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanteteg\Documents\Riverside\Manuscript Updates\Manuscript Changes to Aneta\SNDREV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{590091E6-6948-4ED5-9C06-40F58B489BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E262016E-81D7-42E0-9A28-CA5B8E9C7FD0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF163ACF-DC2B-4606-ADB8-5DB3DA3BF2CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="60" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{83B6147D-AEDB-4F3F-8015-C6928745C0B9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{83B6147D-AEDB-4F3F-8015-C6928745C0B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scheme" sheetId="1" r:id="rId1"/>
     <sheet name="Edit Tracker" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Scheme'!$A$1:$AG$604</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Test Scheme'!$A$1:$AD$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Scheme'!$A$1:$AG$603</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Test Scheme'!$A$1:$AD$29</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="223">
   <si>
     <t>Form</t>
   </si>
@@ -955,15 +955,6 @@
     <t>SNDREV_020</t>
   </si>
   <si>
-    <t>snake</t>
-  </si>
-  <si>
-    <t>snake-canes</t>
-  </si>
-  <si>
-    <t>canes</t>
-  </si>
-  <si>
     <t>23</t>
   </si>
   <si>
@@ -985,9 +976,6 @@
     <t>24</t>
   </si>
   <si>
-    <t>Item 21</t>
-  </si>
-  <si>
     <t>SNDREV_030</t>
   </si>
   <si>
@@ -998,9 +986,6 @@
   </si>
   <si>
     <t>funny</t>
-  </si>
-  <si>
-    <t>25</t>
   </si>
   <si>
     <t xml:space="preserve"> SNDREV_QOP</t>
@@ -1186,6 +1171,12 @@
   </si>
   <si>
     <t>Sample A, Trial 2</t>
+  </si>
+  <si>
+    <t>GJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Based on in info in UAT Tracker and Issues Log and previous AU request (from 4/12/2024), removed Item 19 "snake." Added to list (to the right on this screen). Updated manuscript for a total of 20 test items. Next step: update valid WLookup Score Range to 0-20 in US (JLC). </t>
   </si>
 </sst>
 </file>
@@ -1898,12 +1889,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AG604"/>
+  <dimension ref="A1:AG603"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="N1" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2034,7 +2025,7 @@
         <v>29</v>
       </c>
       <c r="AE1" s="47" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>30</v>
@@ -2066,7 +2057,7 @@
         <v>36</v>
       </c>
       <c r="H2" s="53" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="I2" s="18" t="s">
         <v>37</v>
@@ -2155,7 +2146,7 @@
         <v>41</v>
       </c>
       <c r="H3" s="53" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I3" s="18" t="s">
         <v>42</v>
@@ -2250,7 +2241,7 @@
         <v>51</v>
       </c>
       <c r="H4" s="53" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="I4" s="18" t="s">
         <v>53</v>
@@ -2735,7 +2726,7 @@
         <v>38</v>
       </c>
       <c r="N9" s="25" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="O9" s="29" t="s">
         <v>83</v>
@@ -4030,14 +4021,14 @@
       <c r="A23" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="29" t="s">
         <v>163</v>
       </c>
       <c r="C23" s="45">
-        <v>426908943</v>
+        <v>426908564</v>
       </c>
       <c r="D23" s="48">
-        <v>552953673</v>
+        <v>552961584</v>
       </c>
       <c r="E23" s="31" t="s">
         <v>34</v>
@@ -4045,14 +4036,14 @@
       <c r="F23" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G23" s="18" t="s">
+      <c r="G23" s="31" t="s">
         <v>164</v>
       </c>
       <c r="H23" s="53" t="s">
         <v>164</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="J23" s="44"/>
       <c r="K23" s="18" t="s">
@@ -4065,13 +4056,13 @@
         <v>38</v>
       </c>
       <c r="N23" s="23" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="O23" s="29" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="P23" s="17" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="Q23" s="18" t="s">
         <v>46</v>
@@ -4125,14 +4116,14 @@
       <c r="A24" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>169</v>
+      <c r="B24" s="29" t="s">
+        <v>166</v>
       </c>
       <c r="C24" s="45">
-        <v>426908564</v>
+        <v>426910913</v>
       </c>
       <c r="D24" s="48">
-        <v>552961584</v>
+        <v>552963457</v>
       </c>
       <c r="E24" s="31" t="s">
         <v>34</v>
@@ -4140,14 +4131,14 @@
       <c r="F24" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G24" s="18" t="s">
-        <v>170</v>
+      <c r="G24" s="31" t="s">
+        <v>167</v>
       </c>
       <c r="H24" s="53" t="s">
-        <v>170</v>
-      </c>
-      <c r="I24" s="18" t="s">
-        <v>171</v>
+        <v>167</v>
+      </c>
+      <c r="I24" s="43" t="s">
+        <v>173</v>
       </c>
       <c r="J24" s="44"/>
       <c r="K24" s="18" t="s">
@@ -4160,13 +4151,13 @@
         <v>38</v>
       </c>
       <c r="N24" s="23" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="O24" s="29" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="P24" s="17" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="Q24" s="18" t="s">
         <v>46</v>
@@ -4216,151 +4207,91 @@
       </c>
       <c r="AG24" s="17"/>
     </row>
-    <row r="25" spans="1:33" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="17" t="s">
+    <row r="25" spans="1:33" s="12" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="C25" s="45">
-        <v>426910913</v>
-      </c>
-      <c r="D25" s="48">
-        <v>552963457</v>
-      </c>
-      <c r="E25" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="H25" s="53" t="s">
-        <v>176</v>
-      </c>
-      <c r="I25" s="43" t="s">
+      <c r="B25" s="29" t="s">
+        <v>172</v>
+      </c>
+      <c r="C25" s="30">
+        <v>443231720</v>
+      </c>
+      <c r="D25" s="51" t="s">
+        <v>214</v>
+      </c>
+      <c r="E25" s="31"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="J25" s="44"/>
-      <c r="K25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="L25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="M25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="N25" s="23" t="s">
+      <c r="J25" s="42"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="O25" s="29" t="s">
+      <c r="O25" s="29"/>
+      <c r="P25" s="29"/>
+      <c r="Q25" s="31"/>
+      <c r="R25" s="31"/>
+      <c r="S25" s="31"/>
+      <c r="T25" s="31"/>
+      <c r="U25" s="31"/>
+      <c r="V25" s="31"/>
+      <c r="W25" s="31"/>
+      <c r="X25" s="31"/>
+      <c r="Y25" s="31"/>
+      <c r="Z25" s="31"/>
+      <c r="AA25" s="31"/>
+      <c r="AB25" s="31"/>
+      <c r="AC25" s="31"/>
+      <c r="AD25" s="31"/>
+      <c r="AE25" s="31"/>
+      <c r="AF25" s="31" t="s">
         <v>179</v>
       </c>
-      <c r="P25" s="17" t="s">
+      <c r="AG25" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="Q25" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="R25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="S25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="T25" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="U25" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="V25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="W25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="X25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE25" s="18"/>
-      <c r="AF25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="AG25" s="17"/>
-    </row>
-    <row r="26" spans="1:33" s="12" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="29" t="s">
-        <v>181</v>
-      </c>
-      <c r="C26" s="30">
-        <v>443231720</v>
-      </c>
-      <c r="D26" s="51" t="s">
-        <v>219</v>
-      </c>
-      <c r="E26" s="31"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="41" t="s">
-        <v>182</v>
-      </c>
-      <c r="J26" s="42"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="32" t="s">
-        <v>183</v>
-      </c>
-      <c r="O26" s="29"/>
-      <c r="P26" s="29"/>
-      <c r="Q26" s="31"/>
-      <c r="R26" s="31"/>
-      <c r="S26" s="31"/>
-      <c r="T26" s="31"/>
-      <c r="U26" s="31"/>
-      <c r="V26" s="31"/>
-      <c r="W26" s="31"/>
-      <c r="X26" s="31"/>
-      <c r="Y26" s="31"/>
-      <c r="Z26" s="31"/>
-      <c r="AA26" s="31"/>
-      <c r="AB26" s="31"/>
-      <c r="AC26" s="31"/>
-      <c r="AD26" s="31"/>
-      <c r="AE26" s="31"/>
-      <c r="AF26" s="31" t="s">
-        <v>184</v>
-      </c>
-      <c r="AG26" s="46" t="s">
-        <v>185</v>
-      </c>
+    </row>
+    <row r="26" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
+      <c r="U26" s="12"/>
+      <c r="V26" s="12"/>
+      <c r="W26" s="12"/>
+      <c r="X26" s="12"/>
+      <c r="Y26" s="12"/>
+      <c r="Z26" s="12"/>
+      <c r="AA26" s="12"/>
+      <c r="AB26" s="12"/>
+      <c r="AC26" s="12"/>
+      <c r="AD26" s="12"/>
+      <c r="AE26" s="12"/>
+      <c r="AF26" s="12"/>
+      <c r="AG26" s="12"/>
     </row>
     <row r="27" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10"/>
@@ -4614,33 +4545,12 @@
       <c r="D34" s="49"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="12"/>
-      <c r="P34" s="10"/>
-      <c r="Q34" s="12"/>
-      <c r="R34" s="12"/>
-      <c r="S34" s="12"/>
-      <c r="T34" s="12"/>
-      <c r="U34" s="12"/>
-      <c r="V34" s="12"/>
-      <c r="W34" s="12"/>
-      <c r="X34" s="12"/>
-      <c r="Y34" s="12"/>
-      <c r="Z34" s="12"/>
-      <c r="AA34" s="12"/>
-      <c r="AB34" s="12"/>
-      <c r="AC34" s="12"/>
-      <c r="AD34" s="12"/>
-      <c r="AE34" s="12"/>
-      <c r="AF34" s="12"/>
-      <c r="AG34" s="12"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="N34" s="9"/>
+      <c r="P34" s="11"/>
     </row>
     <row r="35" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="10"/>
@@ -12608,22 +12518,8 @@
       <c r="N603" s="9"/>
       <c r="P603" s="11"/>
     </row>
-    <row r="604" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A604" s="10"/>
-      <c r="B604" s="10"/>
-      <c r="C604" s="10"/>
-      <c r="D604" s="49"/>
-      <c r="E604" s="10"/>
-      <c r="F604" s="10"/>
-      <c r="I604" s="11"/>
-      <c r="J604" s="11"/>
-      <c r="K604" s="11"/>
-      <c r="L604" s="11"/>
-      <c r="N604" s="9"/>
-      <c r="P604" s="11"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:AG604" xr:uid="{889C9C9A-F5C9-4AEE-AFAB-473C7B2118CF}"/>
+  <autoFilter ref="A1:AG603" xr:uid="{889C9C9A-F5C9-4AEE-AFAB-473C7B2118CF}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="27" fitToHeight="0" orientation="landscape" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -12632,11 +12528,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B7561C4-6331-4A7B-80FF-F338DFD70F93}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12653,47 +12549,47 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B2" s="16">
         <v>44319</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B3" s="16">
         <v>44508</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D3" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E3" s="16">
         <v>44510</v>
@@ -12701,16 +12597,16 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B4" s="16">
         <v>44508</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D4" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E4" s="16">
         <v>44510</v>
@@ -12718,16 +12614,16 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B5" s="16">
         <v>44508</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D5" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E5" s="16">
         <v>44510</v>
@@ -12735,36 +12631,36 @@
     </row>
     <row r="6" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B6" s="16">
         <v>44508</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E6" s="16">
         <v>44510</v>
       </c>
       <c r="F6" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B7" s="16">
         <v>44524</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D7" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E7" s="16">
         <v>44529</v>
@@ -12772,16 +12668,16 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B8" s="16">
         <v>44524</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D8" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E8" s="16">
         <v>44529</v>
@@ -12789,16 +12685,16 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B9" s="16">
         <v>44524</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D9" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E9" s="16">
         <v>44529</v>
@@ -12806,16 +12702,16 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B10" s="16">
         <v>44524</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D10" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E10" s="16">
         <v>44529</v>
@@ -12823,16 +12719,16 @@
     </row>
     <row r="11" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B11" s="16">
         <v>44524</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D11" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E11" s="16">
         <v>44529</v>
@@ -12840,16 +12736,16 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B12" s="16">
         <v>44524</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D12" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E12" s="16">
         <v>44529</v>
@@ -12864,29 +12760,29 @@
     </row>
     <row r="14" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B14" s="16">
         <v>45219</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D14" s="33"/>
       <c r="E14" s="33"/>
       <c r="F14" s="13" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B15" s="16">
         <v>45223</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
@@ -12903,13 +12799,13 @@
     </row>
     <row r="16" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B16" s="16">
         <v>45240</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D16" s="33"/>
       <c r="E16" s="33"/>
@@ -12920,19 +12816,19 @@
         <v>92</v>
       </c>
       <c r="H16" s="38" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="M16" s="36"/>
     </row>
     <row r="17" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B17" s="16">
         <v>45245</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F17" s="24">
         <v>426883919</v>
@@ -12941,19 +12837,19 @@
         <v>122</v>
       </c>
       <c r="H17" s="38" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="M17" s="36"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B18" s="16">
         <v>45245</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="F18" s="24">
         <v>426891896</v>
@@ -12962,19 +12858,19 @@
         <v>140</v>
       </c>
       <c r="H18" s="38" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="M18" s="39"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B19" s="16">
         <v>45245</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="F19" s="24">
         <v>426898679</v>
@@ -12983,24 +12879,38 @@
         <v>158</v>
       </c>
       <c r="H19" s="38" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B20" s="16">
         <v>45258</v>
       </c>
       <c r="C20" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="F20" s="45">
+        <v>426908943</v>
+      </c>
+      <c r="G20" s="53" t="s">
+        <v>164</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>221</v>
+      </c>
+      <c r="B21" s="16">
+        <v>45464</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D20" t="s">
-        <v>193</v>
-      </c>
-      <c r="E20" s="16">
-        <v>45259</v>
       </c>
     </row>
   </sheetData>
@@ -13009,12 +12919,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ACB55C607407B649B58320C323E134CB" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c13994d6d2ddba02aa5dd940c3aa9f4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fb8057a2-d102-4556-bf3d-1bd060c1c6e1" xmlns:ns4="3fbd1978-31ec-4369-8fe8-e6440116bc51" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fff83f4678cd9c540a9875a311617aea" ns3:_="" ns4:_="">
     <xsd:import namespace="fb8057a2-d102-4556-bf3d-1bd060c1c6e1"/>
@@ -13237,7 +13141,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -13246,16 +13150,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB7C9551-4A2B-4721-89B5-925D245FA51E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{873E718D-0E51-406D-B7BE-C3027393B741}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13274,10 +13175,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{802F3D32-8F37-45EF-8DEF-C7FB26649453}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB7C9551-4A2B-4721-89B5-925D245FA51E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>